<commit_message>
Modification de la correction au besoin suite aux demandes de recorrection.
</commit_message>
<xml_diff>
--- a/Equipe202.xlsx
+++ b/Equipe202.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22702"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3327\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{B3EACF60-D4C3-4F3D-9DF2-0AC70C608458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A59FAEA-DA86-46E2-AFF3-12DF8FFEF2BD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B57D987E-C299-44E0-8B8F-137DA6DE789F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,8 @@
     <sheet name="Sudoku" sheetId="4" state="hidden" r:id="rId4"/>
     <sheet name="Scrabble" sheetId="5" state="hidden" r:id="rId5"/>
     <sheet name="Sommaire" sheetId="9" r:id="rId6"/>
-    <sheet name="Assurance Qualité" sheetId="6" r:id="rId7"/>
-    <sheet name="Fonctionnalités" sheetId="8" r:id="rId8"/>
+    <sheet name="Fonctionnalités" sheetId="8" r:id="rId7"/>
+    <sheet name="Assurance Qualité" sheetId="6" r:id="rId8"/>
     <sheet name="Curling" sheetId="7" state="hidden" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
@@ -286,19 +286,192 @@
     <t>Grille de correction Projet 2</t>
   </si>
   <si>
+    <t>529f83379738071665f71044e45c70dfcf434309</t>
+  </si>
+  <si>
+    <t>Fonctionnalité</t>
+  </si>
+  <si>
+    <t>Testé</t>
+  </si>
+  <si>
+    <t>Note finale</t>
+  </si>
+  <si>
+    <t>Commentaires</t>
+  </si>
+  <si>
+    <t>Outil-Ligne</t>
+  </si>
+  <si>
+    <t>Test "should call a forced angle if chosen" ne passe pas</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Point d'entrée dans l'application</t>
+  </si>
+  <si>
+    <t>Antoine Labonté</t>
+  </si>
+  <si>
+    <t>Vue de dessin</t>
+  </si>
+  <si>
+    <t>On ne voit pas quel outil est sélectionné juste en regardant les icônes.</t>
+  </si>
+  <si>
+    <t>Créer un nouveau dessin</t>
+  </si>
+  <si>
+    <t>L'application lance une erreur lorsqu’on tente d’afficher deux modals de création.
+Il est possible de faire tous les raccourcis lorsque la modal est affichée.
+Il n’existe pas de palette de couleur pour choisir la couleur d’arrière plan. Seulement des couleurs prédéfinies.
+Lorsqu’on redimension l’application après l’apparition du modal les valeurs ne se mettent pas à jour.
+Test "NewDrawComponent should close modal window on cancel" ne passe pas</t>
+  </si>
+  <si>
+    <t>Outil-Couleur</t>
+  </si>
+  <si>
+    <t>On ne peut pas modifier la couleur lorsqu’on est dans les paramètres d’un outil autre que le selectionneur de couleur.
+On peut définir la transparence, mais on ne peut pas l’appliquer. Les outils ne font plus rien.
+On ne peut pas modifier la couleur de l’arrière plan une fois le dessin créé.
+On ne peut pas spécifier une couleur en utilisant des valeurs hexadécimales.[OK]
+Les couleurs du bas du cercle ne réflètent pas la couleur attendue.
+Quatre tests dont 2 dans ColorPickingService et dans ColorConvertingService ne passe pas et certaines branches ne sont pas atteintes dans ces fichiers.</t>
+  </si>
+  <si>
+    <t>Antoine Lamontagne</t>
+  </si>
+  <si>
+    <t>Outil-Rectangle</t>
+  </si>
+  <si>
+    <t>Attention, la phrase "should not update the drawing of the tool change is on-the-fly" serait à retravailler</t>
+  </si>
+  <si>
+    <t>Outil-Pinceau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vos textures se ressemblent beaucoup, il serait bien de les diversifier. (Bruit 1, 2, 3 et 4) [OK]
+On continue de dessiner si le curseur sort de la zone de dessin. [OK]
+</t>
+  </si>
+  <si>
+    <t>Outil-Crayon</t>
+  </si>
+  <si>
+    <t>On continue de dessiner si le curseur sort de la zone de dessin. [OK]</t>
+  </si>
+  <si>
+    <t>Guide d'utilisation</t>
+  </si>
+  <si>
+    <t>Mauvais nom de test "should stay at the same page at the last page when calling previousPage". Les branches (if) ne sont pas couvertes dans nextPage() et previousPage(), ce sont les parties critiques de votre logique de changement de page.</t>
+  </si>
+  <si>
+    <t>Note finale pour le sprint</t>
+  </si>
+  <si>
+    <t>Crash</t>
+  </si>
+  <si>
+    <t>Ne build pas</t>
+  </si>
+  <si>
+    <t>Annuler-refaire</t>
+  </si>
+  <si>
+    <t>Sauvegarder le dessin sur serveur</t>
+  </si>
+  <si>
+    <t>Galerie de dessins</t>
+  </si>
+  <si>
+    <t>Base de données</t>
+  </si>
+  <si>
+    <t>Filtrage par étiquettes</t>
+  </si>
+  <si>
+    <t>Exporter le dessin</t>
+  </si>
+  <si>
+    <t>Outil-Sélection et inversion de sélection</t>
+  </si>
+  <si>
+    <t>Déplacement d'une sélection</t>
+  </si>
+  <si>
+    <t>Outil-Efface</t>
+  </si>
+  <si>
+    <t>Outi-Pipette</t>
+  </si>
+  <si>
+    <t>Outil-Applicateur de couleur</t>
+  </si>
+  <si>
+    <t>Outil-Aérosol</t>
+  </si>
+  <si>
+    <t>Outil-Polygone</t>
+  </si>
+  <si>
+    <t>Outil-Ellipse</t>
+  </si>
+  <si>
+    <t>Grille</t>
+  </si>
+  <si>
+    <t>Guide d'utilisation - mise à jour</t>
+  </si>
+  <si>
+    <t>Anciennes fonctionnalités brisées</t>
+  </si>
+  <si>
+    <t>Continuer un dessin</t>
+  </si>
+  <si>
+    <t>Sauvegarde automatique</t>
+  </si>
+  <si>
+    <t>Outil-Texte</t>
+  </si>
+  <si>
+    <t>Outil-Plume</t>
+  </si>
+  <si>
+    <t>Outil-Étampe</t>
+  </si>
+  <si>
+    <t>Outil-Sceau de peinute</t>
+  </si>
+  <si>
+    <t>Magnétisme (surface de dessin)</t>
+  </si>
+  <si>
+    <t>Redimensionnement d'une sélection</t>
+  </si>
+  <si>
+    <t>Rotation d'une sélection</t>
+  </si>
+  <si>
+    <t>Manipulations de sélections et presse-papier</t>
+  </si>
+  <si>
+    <t>Envoyer le dessin par courriel</t>
+  </si>
+  <si>
     <t>Critère</t>
   </si>
   <si>
-    <t>Commentaires</t>
-  </si>
-  <si>
     <t>Poid</t>
   </si>
   <si>
     <t>Qualité des classes</t>
-  </si>
-  <si>
-    <t>Antoine Labonté</t>
   </si>
   <si>
     <t>La classe n'a qu'une responsabilitée et elle est non triviale. Son nom est court, clair pertinent et représentatif de sa responsabilité. La classe ne contient que l'information qu'elle nécessite (idéalement moins de 7 attributs)</t>
@@ -353,9 +526,6 @@
     <t>Exceptions</t>
   </si>
   <si>
-    <t>Antoine Lamontagne</t>
-  </si>
-  <si>
     <t>Les exceptions sont claires et spécifiques (Pas d'erreurs génériques)</t>
   </si>
   <si>
@@ -381,9 +551,6 @@
   </si>
   <si>
     <t>Expression Booléennes</t>
-  </si>
-  <si>
-    <t>William</t>
   </si>
   <si>
     <t>Les expression booléennes ne sont pas comparées à true et false</t>
@@ -468,7 +635,7 @@
     <t>Chaque commit concerne une seule "issue" et les messages sont pertinents et suffisamment descriptifs pour chaque commit</t>
   </si>
   <si>
-    <t>Il n'y a aucune convention de nommage qui est suivie lors de la création de vos branches.</t>
+    <t>Il n'y a aucune convention de nommage qui est suivie lors de la création de vos branches. [OK]</t>
   </si>
   <si>
     <t>Le repo git ne contient que les fichiers nécessaires. (pas de dossier node_modules ou de package-lock.json et pas de package.json dans des dossiers autre que client ou server)</t>
@@ -478,173 +645,6 @@
   </si>
   <si>
     <t>Note assurance qualité</t>
-  </si>
-  <si>
-    <t>529f83379738071665f71044e45c70dfcf434309</t>
-  </si>
-  <si>
-    <t>Fonctionnalité</t>
-  </si>
-  <si>
-    <t>Testé</t>
-  </si>
-  <si>
-    <t>Note finale</t>
-  </si>
-  <si>
-    <t>Outil-Ligne</t>
-  </si>
-  <si>
-    <t>Test "should call a forced angle if chosen" ne passe pas</t>
-  </si>
-  <si>
-    <t>Point d'entrée dans l'application</t>
-  </si>
-  <si>
-    <t>Vue de dessin</t>
-  </si>
-  <si>
-    <t>On ne voit pas quel outil est sélectionné juste en regardant les icônes.</t>
-  </si>
-  <si>
-    <t>Créer un nouveau dessin</t>
-  </si>
-  <si>
-    <t>L'application lance une erreur lorsqu’on tente d’afficher deux modals de création.
-Il est possible de faire tous les raccourcis lorsque la modal est affichée.
-Il n’existe pas de palette de couleur pour choisir la couleur d’arrière plan. Seulement des couleurs prédéfinies.
-Lorsqu’on redimension l’application après l’apparition du modal les valeurs ne se mettent pas à jour.
-Test "NewDrawComponent should close modal window on cancel" ne passe pas</t>
-  </si>
-  <si>
-    <t>Outil-Couleur</t>
-  </si>
-  <si>
-    <t>On ne peut pas modifier la couleur lorsqu’on est dans les paramètres d’un outil autre que le selectionneur de couleur.
-On peut définir la transparence, mais on ne peut pas l’appliquer. Les outils ne font plus rien.
-On ne peut pas modifier la couleur de l’arrière plan une fois le dessin créé.
-On ne peut pas spécifier une couleur en utilisant des valeurs hexadécimales.
-Les couleurs du bas du cercle ne réflètent pas la couleur attendue.
-Quatre tests dont 2 dans ColorPickingService et dans ColorConvertingService ne passe pas et certaines branches ne sont pas atteintes dans ces fichiers.</t>
-  </si>
-  <si>
-    <t>Outil-Rectangle</t>
-  </si>
-  <si>
-    <t>Attention, la phrase "should not update the drawing of the tool change is on-the-fly" serait à retravailler</t>
-  </si>
-  <si>
-    <t>Outil-Pinceau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vos textures se ressemblent beaucoup, il serait bien de les diversifier. (Bruit 1, 2, 3 et 4)
-On continue de dessiner si le curseur sort de la zone de dessin.
-</t>
-  </si>
-  <si>
-    <t>Outil-Crayon</t>
-  </si>
-  <si>
-    <t>On continue de dessiner si le curseur sort de la zone de dessin.</t>
-  </si>
-  <si>
-    <t>Guide d'utilisation</t>
-  </si>
-  <si>
-    <t>Mauvais nom de test "should stay at the same page at the last page when calling previousPage". Les branches (if) ne sont pas couvertes dans nextPage() et previousPage(), ce sont les parties critiques de votre logique de changement de page.</t>
-  </si>
-  <si>
-    <t>Note finale pour le sprint</t>
-  </si>
-  <si>
-    <t>Crash</t>
-  </si>
-  <si>
-    <t>Ne build pas</t>
-  </si>
-  <si>
-    <t>Annuler-refaire</t>
-  </si>
-  <si>
-    <t>Sauvegarder le dessin sur serveur</t>
-  </si>
-  <si>
-    <t>Galerie de dessins</t>
-  </si>
-  <si>
-    <t>Base de données</t>
-  </si>
-  <si>
-    <t>Filtrage par étiquettes</t>
-  </si>
-  <si>
-    <t>Exporter le dessin</t>
-  </si>
-  <si>
-    <t>Outil-Sélection et inversion de sélection</t>
-  </si>
-  <si>
-    <t>Déplacement d'une sélection</t>
-  </si>
-  <si>
-    <t>Outil-Efface</t>
-  </si>
-  <si>
-    <t>Outi-Pipette</t>
-  </si>
-  <si>
-    <t>Outil-Applicateur de couleur</t>
-  </si>
-  <si>
-    <t>Outil-Aérosol</t>
-  </si>
-  <si>
-    <t>Outil-Polygone</t>
-  </si>
-  <si>
-    <t>Outil-Ellipse</t>
-  </si>
-  <si>
-    <t>Grille</t>
-  </si>
-  <si>
-    <t>Guide d'utilisation - mise à jour</t>
-  </si>
-  <si>
-    <t>Anciennes fonctionnalités brisées</t>
-  </si>
-  <si>
-    <t>Continuer un dessin</t>
-  </si>
-  <si>
-    <t>Sauvegarde automatique</t>
-  </si>
-  <si>
-    <t>Outil-Texte</t>
-  </si>
-  <si>
-    <t>Outil-Plume</t>
-  </si>
-  <si>
-    <t>Outil-Étampe</t>
-  </si>
-  <si>
-    <t>Outil-Sceau de peinute</t>
-  </si>
-  <si>
-    <t>Magnétisme (surface de dessin)</t>
-  </si>
-  <si>
-    <t>Redimensionnement d'une sélection</t>
-  </si>
-  <si>
-    <t>Rotation d'une sélection</t>
-  </si>
-  <si>
-    <t>Manipulations de sélections et presse-papier</t>
-  </si>
-  <si>
-    <t>Envoyer le dessin par courriel</t>
   </si>
   <si>
     <t>Implémentation d’un joueur virtuel avec deux niveaux: facile et difficile</t>
@@ -3566,69 +3566,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="102" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="11" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="11" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3678,6 +3615,69 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="102" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6281,22 +6281,22 @@
       </c>
       <c r="B4" s="268">
         <f>(Fonctionnalités!E17)</f>
-        <v>0.75700000000000001</v>
+        <v>0.79349999999999998</v>
       </c>
       <c r="C4" s="269">
         <f>'Assurance Qualité'!B49</f>
-        <v>0.51849999999999996</v>
+        <v>0.53849999999999998</v>
       </c>
       <c r="D4" s="269">
         <f>AVERAGE(B4:C4) - 0.1*E4</f>
-        <v>0.63775000000000004</v>
+        <v>0.66599999999999993</v>
       </c>
       <c r="F4" s="280">
         <v>15</v>
       </c>
       <c r="G4" s="279">
         <f>D4*F4</f>
-        <v>9.5662500000000001</v>
+        <v>9.9899999999999984</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6368,11 +6368,954 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A54262-C76A-40FE-9AF3-642EF9B2EA00}">
+  <dimension ref="A1:G61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="73" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="89.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75">
+      <c r="A1" s="300" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="301"/>
+      <c r="C1" s="301"/>
+      <c r="D1" s="301"/>
+      <c r="E1" s="301"/>
+      <c r="F1" s="301"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="218"/>
+      <c r="B2" s="218"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="218"/>
+      <c r="F2" s="219"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.75">
+      <c r="A3" s="300" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="301"/>
+      <c r="C3" s="301"/>
+      <c r="D3" s="301"/>
+      <c r="E3" s="301"/>
+      <c r="F3" s="301"/>
+    </row>
+    <row r="5" spans="1:7" ht="23.25">
+      <c r="A5" s="302" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="302"/>
+      <c r="C5" s="302"/>
+      <c r="D5" s="302"/>
+      <c r="E5" s="302"/>
+      <c r="F5" s="302"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="220" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="303" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="303"/>
+      <c r="D6" s="303"/>
+      <c r="E6" s="303"/>
+      <c r="F6" s="304"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="221" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="222" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="222" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="222" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="222" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="223" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="224" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="225">
+        <v>1</v>
+      </c>
+      <c r="C8" s="225">
+        <v>0.75</v>
+      </c>
+      <c r="D8" s="225">
+        <v>16</v>
+      </c>
+      <c r="E8" s="225">
+        <f t="shared" ref="E8:E13" si="0">B8*C8*D8</f>
+        <v>12</v>
+      </c>
+      <c r="F8" s="284" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="282" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="224" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="225">
+        <v>1</v>
+      </c>
+      <c r="C9" s="225">
+        <v>1</v>
+      </c>
+      <c r="D9" s="225">
+        <v>8</v>
+      </c>
+      <c r="E9" s="225">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F9" s="285"/>
+      <c r="G9" s="282" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="224" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="225">
+        <v>0.85</v>
+      </c>
+      <c r="C10" s="225">
+        <v>1</v>
+      </c>
+      <c r="D10" s="225">
+        <v>10</v>
+      </c>
+      <c r="E10" s="225">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="F10" s="285" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" s="282" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="105">
+      <c r="A11" s="224" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="225">
+        <v>0.65</v>
+      </c>
+      <c r="C11" s="225">
+        <v>0.75</v>
+      </c>
+      <c r="D11" s="225">
+        <v>12</v>
+      </c>
+      <c r="E11" s="225">
+        <f t="shared" si="0"/>
+        <v>5.8500000000000005</v>
+      </c>
+      <c r="F11" s="284" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="282" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="120">
+      <c r="A12" s="224" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="225">
+        <v>0.7</v>
+      </c>
+      <c r="C12" s="225">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="225">
+        <v>10</v>
+      </c>
+      <c r="E12" s="225">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="F12" s="284" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="282" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30">
+      <c r="A13" s="224" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="225">
+        <v>1</v>
+      </c>
+      <c r="C13" s="225">
+        <v>1</v>
+      </c>
+      <c r="D13" s="225">
+        <v>12</v>
+      </c>
+      <c r="E13" s="225">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F13" s="284" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="282" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45">
+      <c r="A14" s="224" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="225">
+        <v>1</v>
+      </c>
+      <c r="C14" s="225">
+        <v>1</v>
+      </c>
+      <c r="D14" s="225">
+        <v>12</v>
+      </c>
+      <c r="E14" s="225">
+        <f t="shared" ref="E14:E16" si="1">B14*C14*D14</f>
+        <v>12</v>
+      </c>
+      <c r="F14" s="284" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="282" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="224" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="225">
+        <v>1</v>
+      </c>
+      <c r="C15" s="225">
+        <v>1</v>
+      </c>
+      <c r="D15" s="225">
+        <v>10</v>
+      </c>
+      <c r="E15" s="225">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F15" s="285" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="282" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="224" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="225">
+        <v>1</v>
+      </c>
+      <c r="C16" s="225">
+        <v>0.75</v>
+      </c>
+      <c r="D16" s="225">
+        <v>10</v>
+      </c>
+      <c r="E16" s="225">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="F16" s="285" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="282" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="226" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="305"/>
+      <c r="C17" s="305"/>
+      <c r="D17" s="286">
+        <f>SUM(D8:D16)</f>
+        <v>100</v>
+      </c>
+      <c r="E17" s="278">
+        <f>SUM(E8:E16)/D17 - E19*D19 - E18*D18</f>
+        <v>0.79349999999999998</v>
+      </c>
+      <c r="F17" s="227"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="228" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="229">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="228" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="229">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="23.25">
+      <c r="A20" s="306" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="307"/>
+      <c r="C20" s="307"/>
+      <c r="D20" s="307"/>
+      <c r="E20" s="307"/>
+      <c r="F20" s="308"/>
+    </row>
+    <row r="21" spans="1:6" ht="25.5" customHeight="1">
+      <c r="A21" s="238" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="292"/>
+      <c r="C21" s="293"/>
+      <c r="D21" s="293"/>
+      <c r="E21" s="293"/>
+      <c r="F21" s="294"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="238" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="230" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="230" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="230" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="230" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="239" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="238" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="252"/>
+      <c r="C23" s="252"/>
+      <c r="D23" s="230">
+        <v>12</v>
+      </c>
+      <c r="E23" s="230">
+        <f>B23*C23*D23</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="239"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="238" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="252"/>
+      <c r="C24" s="252"/>
+      <c r="D24" s="230">
+        <v>8</v>
+      </c>
+      <c r="E24" s="230">
+        <f>B24*C24*D24</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="239"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="238" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="252"/>
+      <c r="C25" s="252"/>
+      <c r="D25" s="230">
+        <v>8</v>
+      </c>
+      <c r="E25" s="230">
+        <f>B25*C25*D25</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="239"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="238" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="252"/>
+      <c r="C26" s="252"/>
+      <c r="D26" s="230">
+        <v>4</v>
+      </c>
+      <c r="E26" s="230">
+        <f>B26*C26*D26</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="239"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="238" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="252"/>
+      <c r="C27" s="252"/>
+      <c r="D27" s="230">
+        <v>5</v>
+      </c>
+      <c r="E27" s="230">
+        <f>B27*C27*D27</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="239"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="238" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="252"/>
+      <c r="C28" s="252"/>
+      <c r="D28" s="230">
+        <v>5</v>
+      </c>
+      <c r="E28" s="230">
+        <f t="shared" ref="E28:E38" si="2">B28*C28*D28</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="239"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="238" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="252"/>
+      <c r="C29" s="252"/>
+      <c r="D29" s="230">
+        <v>14</v>
+      </c>
+      <c r="E29" s="230">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="239"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="238" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="252"/>
+      <c r="C30" s="252"/>
+      <c r="D30" s="230">
+        <v>6</v>
+      </c>
+      <c r="E30" s="230">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="239"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="238" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="252"/>
+      <c r="C31" s="252"/>
+      <c r="D31" s="230">
+        <v>8</v>
+      </c>
+      <c r="E31" s="230">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="239"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="238" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="252"/>
+      <c r="C32" s="252"/>
+      <c r="D32" s="230">
+        <v>4</v>
+      </c>
+      <c r="E32" s="230">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="239"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="238" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" s="252"/>
+      <c r="C33" s="252"/>
+      <c r="D33" s="230">
+        <v>4</v>
+      </c>
+      <c r="E33" s="230">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="239"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="251" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" s="252"/>
+      <c r="C34" s="252"/>
+      <c r="D34" s="252">
+        <v>6</v>
+      </c>
+      <c r="E34" s="230">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="253"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="251" t="s">
+        <v>121</v>
+      </c>
+      <c r="B35" s="252"/>
+      <c r="C35" s="252"/>
+      <c r="D35" s="252">
+        <v>6</v>
+      </c>
+      <c r="E35" s="230">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="253"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="251" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" s="252"/>
+      <c r="C36" s="252"/>
+      <c r="D36" s="252">
+        <v>4</v>
+      </c>
+      <c r="E36" s="230">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="253"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="251" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" s="252"/>
+      <c r="C37" s="252"/>
+      <c r="D37" s="252">
+        <v>4</v>
+      </c>
+      <c r="E37" s="230">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="253"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="251" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" s="252"/>
+      <c r="C38" s="252"/>
+      <c r="D38" s="252">
+        <v>2</v>
+      </c>
+      <c r="E38" s="230">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="253"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="240" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="241"/>
+      <c r="C39" s="262"/>
+      <c r="D39" s="262">
+        <f>SUM(D23:D38)</f>
+        <v>100</v>
+      </c>
+      <c r="E39" s="242">
+        <f>SUM(E23:E38)/D39 -E40*D40 -E41*D41-E42*D42</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="243"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="231" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="264"/>
+      <c r="D40" s="263">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="231" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" s="232">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="231" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" s="233">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="23.25">
+      <c r="A43" s="295" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="296"/>
+      <c r="C43" s="296"/>
+      <c r="D43" s="296"/>
+      <c r="E43" s="296"/>
+      <c r="F43" s="297"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="244" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="298"/>
+      <c r="C44" s="298"/>
+      <c r="D44" s="298"/>
+      <c r="E44" s="298"/>
+      <c r="F44" s="299"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="245" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="234" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="234" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="234" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="234" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="246" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="247" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46" s="235"/>
+      <c r="C46" s="235"/>
+      <c r="D46" s="235">
+        <v>5</v>
+      </c>
+      <c r="E46" s="235">
+        <f t="shared" ref="E46:E52" si="3">B46*C46*D46</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="246"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="247" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" s="235"/>
+      <c r="C47" s="235"/>
+      <c r="D47" s="235">
+        <v>10</v>
+      </c>
+      <c r="E47" s="235">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F47" s="248"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="247" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" s="235"/>
+      <c r="C48" s="235"/>
+      <c r="D48" s="235">
+        <v>8</v>
+      </c>
+      <c r="E48" s="235">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="246"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="247" t="s">
+        <v>129</v>
+      </c>
+      <c r="B49" s="235"/>
+      <c r="C49" s="235"/>
+      <c r="D49" s="235">
+        <v>6</v>
+      </c>
+      <c r="E49" s="235">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="248"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="247" t="s">
+        <v>130</v>
+      </c>
+      <c r="B50" s="235"/>
+      <c r="C50" s="235"/>
+      <c r="D50" s="235">
+        <v>6</v>
+      </c>
+      <c r="E50" s="235">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="246"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="247" t="s">
+        <v>131</v>
+      </c>
+      <c r="B51" s="235"/>
+      <c r="C51" s="235"/>
+      <c r="D51" s="235">
+        <v>15</v>
+      </c>
+      <c r="E51" s="235">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="246"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="247" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" s="235"/>
+      <c r="C52" s="235"/>
+      <c r="D52" s="235">
+        <v>8</v>
+      </c>
+      <c r="E52" s="235">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="246"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="247" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="255"/>
+      <c r="C53" s="255"/>
+      <c r="D53" s="235">
+        <v>12</v>
+      </c>
+      <c r="E53" s="235">
+        <f t="shared" ref="E53:E57" si="4">B53*C53*D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="246"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="259" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="257"/>
+      <c r="C54" s="257"/>
+      <c r="D54" s="254">
+        <v>12</v>
+      </c>
+      <c r="E54" s="235">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="256"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="259" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="257"/>
+      <c r="C55" s="257"/>
+      <c r="D55" s="254">
+        <v>12</v>
+      </c>
+      <c r="E55" s="235">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="256"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="259" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="257"/>
+      <c r="C56" s="257"/>
+      <c r="D56" s="254">
+        <v>4</v>
+      </c>
+      <c r="E56" s="235">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="256"/>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="259" t="s">
+        <v>124</v>
+      </c>
+      <c r="B57" s="257"/>
+      <c r="C57" s="257"/>
+      <c r="D57" s="254">
+        <v>2</v>
+      </c>
+      <c r="E57" s="235">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="256"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="260" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" s="258"/>
+      <c r="C58" s="258"/>
+      <c r="D58" s="261">
+        <f>SUM(D46:D57)</f>
+        <v>100</v>
+      </c>
+      <c r="E58" s="249">
+        <f>SUM(E46:E57)/D58 - D59*E59  - D60*E60 - D61*E61</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="250"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="236" t="s">
+        <v>107</v>
+      </c>
+      <c r="D59" s="232">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="236" t="s">
+        <v>108</v>
+      </c>
+      <c r="D60" s="232">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="237" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" s="233">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A20:F20"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B17 B46:B57" xr:uid="{CC44C972-8B8F-4678-BAEB-D51FFB0200E2}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C16 C18 C46:C57" xr:uid="{DCFB5783-098F-4837-84E1-A329359B138C}">
+      <formula1>"0,0.25,0.50,0.75,1"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E19 E41 E60" xr:uid="{301E7E41-CD71-4A91-B881-91EF87706901}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6388,15 +7331,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A1" s="299" t="s">
+      <c r="A1" s="316" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="300"/>
-      <c r="C1" s="300"/>
-      <c r="D1" s="300"/>
-      <c r="E1" s="300"/>
-      <c r="F1" s="300"/>
-      <c r="G1" s="301"/>
+      <c r="B1" s="317"/>
+      <c r="C1" s="317"/>
+      <c r="D1" s="317"/>
+      <c r="E1" s="317"/>
+      <c r="F1" s="317"/>
+      <c r="G1" s="318"/>
       <c r="H1" s="217"/>
       <c r="I1" s="217"/>
     </row>
@@ -6405,15 +7348,15 @@
       <c r="I2" s="200"/>
     </row>
     <row r="3" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A3" s="302" t="s">
+      <c r="A3" s="319" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="303"/>
-      <c r="C3" s="303"/>
-      <c r="D3" s="303"/>
-      <c r="E3" s="303"/>
-      <c r="F3" s="303"/>
-      <c r="G3" s="304"/>
+      <c r="B3" s="320"/>
+      <c r="C3" s="320"/>
+      <c r="D3" s="320"/>
+      <c r="E3" s="320"/>
+      <c r="F3" s="320"/>
+      <c r="G3" s="321"/>
       <c r="H3" s="196"/>
       <c r="I3" s="196"/>
     </row>
@@ -6429,48 +7372,48 @@
       <c r="I4" s="146"/>
     </row>
     <row r="5" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A5" s="307" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="309" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="309"/>
-      <c r="D5" s="310" t="s">
+      <c r="A5" s="324" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="326" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="326"/>
+      <c r="D5" s="327" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="310"/>
-      <c r="F5" s="311" t="s">
+      <c r="E5" s="327"/>
+      <c r="F5" s="328" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="312"/>
+      <c r="G5" s="329"/>
       <c r="H5" s="195"/>
       <c r="I5" s="195"/>
-      <c r="J5" s="305" t="s">
-        <v>82</v>
-      </c>
-      <c r="K5" s="306"/>
-      <c r="L5" s="306"/>
+      <c r="J5" s="322" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="323"/>
+      <c r="L5" s="323"/>
     </row>
     <row r="6" spans="1:13" ht="18.75">
-      <c r="A6" s="308"/>
+      <c r="A6" s="325"/>
       <c r="B6" s="147" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="148" t="s">
-        <v>83</v>
+        <v>138</v>
       </c>
       <c r="D6" s="149" t="s">
         <v>48</v>
       </c>
       <c r="E6" s="150" t="s">
-        <v>83</v>
+        <v>138</v>
       </c>
       <c r="F6" s="151" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="202" t="s">
-        <v>83</v>
+        <v>138</v>
       </c>
       <c r="H6" s="195"/>
       <c r="I6" s="195"/>
@@ -6486,23 +7429,23 @@
       <c r="M6" s="152"/>
     </row>
     <row r="7" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A7" s="292" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="293"/>
-      <c r="C7" s="293"/>
-      <c r="D7" s="293"/>
-      <c r="E7" s="293"/>
-      <c r="F7" s="293"/>
-      <c r="G7" s="294"/>
+      <c r="A7" s="309" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="310"/>
+      <c r="C7" s="310"/>
+      <c r="D7" s="310"/>
+      <c r="E7" s="310"/>
+      <c r="F7" s="310"/>
+      <c r="G7" s="311"/>
       <c r="H7" s="196" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I7" s="196"/>
     </row>
     <row r="8" spans="1:13" ht="71.25" customHeight="1">
       <c r="A8" s="203" t="s">
-        <v>86</v>
+        <v>140</v>
       </c>
       <c r="B8" s="153">
         <v>0.6</v>
@@ -6521,12 +7464,12 @@
       <c r="H8" s="197"/>
       <c r="I8" s="197"/>
       <c r="J8" s="1" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15">
       <c r="A9" s="205" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
       <c r="B9" s="158">
         <v>0</v>
@@ -6545,12 +7488,12 @@
       <c r="H9" s="197"/>
       <c r="I9" s="197"/>
       <c r="J9" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15">
       <c r="A10" s="207" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="B10" s="158">
         <v>0.9</v>
@@ -6569,12 +7512,12 @@
       <c r="H10" s="197"/>
       <c r="I10" s="197"/>
       <c r="J10" s="1" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15">
       <c r="A11" s="209" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="B11" s="187">
         <f>SUMPRODUCT(B8:B10,C8:C10)</f>
@@ -6604,23 +7547,23 @@
       <c r="I11" s="197"/>
     </row>
     <row r="12" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A12" s="292" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="293"/>
-      <c r="C12" s="293"/>
-      <c r="D12" s="293"/>
-      <c r="E12" s="293"/>
-      <c r="F12" s="293"/>
-      <c r="G12" s="294"/>
+      <c r="A12" s="309" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" s="310"/>
+      <c r="C12" s="310"/>
+      <c r="D12" s="310"/>
+      <c r="E12" s="310"/>
+      <c r="F12" s="310"/>
+      <c r="G12" s="311"/>
       <c r="H12" s="196" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I12" s="196"/>
     </row>
     <row r="13" spans="1:13" ht="45">
       <c r="A13" s="203" t="s">
-        <v>94</v>
+        <v>148</v>
       </c>
       <c r="B13" s="168">
         <v>0.7</v>
@@ -6639,12 +7582,12 @@
       <c r="H13" s="198"/>
       <c r="I13" s="197"/>
       <c r="J13" s="1" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30">
       <c r="A14" s="205" t="s">
-        <v>96</v>
+        <v>150</v>
       </c>
       <c r="B14" s="171">
         <v>1</v>
@@ -6665,7 +7608,7 @@
     </row>
     <row r="15" spans="1:13" ht="15">
       <c r="A15" s="205" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="B15" s="171">
         <v>1</v>
@@ -6686,7 +7629,7 @@
     </row>
     <row r="16" spans="1:13" ht="60">
       <c r="A16" s="207" t="s">
-        <v>98</v>
+        <v>152</v>
       </c>
       <c r="B16" s="174">
         <v>0.75</v>
@@ -6705,12 +7648,12 @@
       <c r="H16" s="198"/>
       <c r="I16" s="197"/>
       <c r="J16" s="1" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15">
       <c r="A17" s="209" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="B17" s="187">
         <f>SUMPRODUCT(B13:B16,C13:C16)</f>
@@ -6740,23 +7683,23 @@
       <c r="I17" s="197"/>
     </row>
     <row r="18" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A18" s="292" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="293"/>
-      <c r="C18" s="293"/>
-      <c r="D18" s="293"/>
-      <c r="E18" s="293"/>
-      <c r="F18" s="293"/>
-      <c r="G18" s="294"/>
+      <c r="A18" s="309" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" s="310"/>
+      <c r="C18" s="310"/>
+      <c r="D18" s="310"/>
+      <c r="E18" s="310"/>
+      <c r="F18" s="310"/>
+      <c r="G18" s="311"/>
       <c r="H18" s="196" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I18" s="196"/>
     </row>
     <row r="19" spans="1:10" ht="15">
       <c r="A19" s="205" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
       <c r="B19" s="158">
         <v>1</v>
@@ -6777,7 +7720,7 @@
     </row>
     <row r="20" spans="1:10" ht="15">
       <c r="A20" s="207" t="s">
-        <v>103</v>
+        <v>156</v>
       </c>
       <c r="B20" s="158">
         <v>1</v>
@@ -6798,7 +7741,7 @@
     </row>
     <row r="21" spans="1:10" ht="15">
       <c r="A21" s="209" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="B21" s="187">
         <f>SUMPRODUCT(B19:B20,C19:C20)</f>
@@ -6828,23 +7771,23 @@
       <c r="I21" s="197"/>
     </row>
     <row r="22" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A22" s="292" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" s="293"/>
-      <c r="C22" s="293"/>
-      <c r="D22" s="293"/>
-      <c r="E22" s="293"/>
-      <c r="F22" s="293"/>
-      <c r="G22" s="294"/>
+      <c r="A22" s="309" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" s="310"/>
+      <c r="C22" s="310"/>
+      <c r="D22" s="310"/>
+      <c r="E22" s="310"/>
+      <c r="F22" s="310"/>
+      <c r="G22" s="311"/>
       <c r="H22" s="196" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I22" s="196"/>
     </row>
     <row r="23" spans="1:10" ht="30">
       <c r="A23" s="207" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
       <c r="B23" s="171">
         <v>0.5</v>
@@ -6863,12 +7806,12 @@
       <c r="H23" s="198"/>
       <c r="I23" s="197"/>
       <c r="J23" s="1" t="s">
-        <v>106</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="45">
       <c r="A24" s="207" t="s">
-        <v>107</v>
+        <v>160</v>
       </c>
       <c r="B24" s="171">
         <v>0.4</v>
@@ -6887,12 +7830,12 @@
       <c r="H24" s="198"/>
       <c r="I24" s="197"/>
       <c r="J24" s="1" t="s">
-        <v>108</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15">
       <c r="A25" s="209" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="B25" s="187">
         <f>SUMPRODUCT(B23:B24,C23:C24)</f>
@@ -6922,23 +7865,23 @@
       <c r="I25" s="197"/>
     </row>
     <row r="26" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A26" s="292" t="s">
-        <v>109</v>
-      </c>
-      <c r="B26" s="293"/>
-      <c r="C26" s="293"/>
-      <c r="D26" s="293"/>
-      <c r="E26" s="293"/>
-      <c r="F26" s="293"/>
-      <c r="G26" s="294"/>
+      <c r="A26" s="309" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="310"/>
+      <c r="C26" s="310"/>
+      <c r="D26" s="310"/>
+      <c r="E26" s="310"/>
+      <c r="F26" s="310"/>
+      <c r="G26" s="311"/>
       <c r="H26" s="196" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="I26" s="196"/>
     </row>
     <row r="27" spans="1:10" ht="15">
       <c r="A27" s="203" t="s">
-        <v>111</v>
+        <v>163</v>
       </c>
       <c r="B27" s="178">
         <v>0</v>
@@ -6957,12 +7900,12 @@
       <c r="H27" s="198"/>
       <c r="I27" s="197"/>
       <c r="J27" t="s">
-        <v>112</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="30">
       <c r="A28" s="205" t="s">
-        <v>113</v>
+        <v>165</v>
       </c>
       <c r="B28" s="171">
         <v>0.5</v>
@@ -6981,12 +7924,12 @@
       <c r="H28" s="198"/>
       <c r="I28" s="197"/>
       <c r="J28" s="1" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30">
       <c r="A29" s="207" t="s">
-        <v>115</v>
+        <v>167</v>
       </c>
       <c r="B29" s="171">
         <v>1</v>
@@ -7007,7 +7950,7 @@
     </row>
     <row r="30" spans="1:10" ht="15">
       <c r="A30" s="209" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="B30" s="181">
         <f>SUMPRODUCT(B27:B29,C27:C29)</f>
@@ -7037,23 +7980,23 @@
       <c r="I30" s="197"/>
     </row>
     <row r="31" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A31" s="292" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" s="293"/>
-      <c r="C31" s="293"/>
-      <c r="D31" s="293"/>
-      <c r="E31" s="293"/>
-      <c r="F31" s="293"/>
-      <c r="G31" s="294"/>
+      <c r="A31" s="309" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31" s="310"/>
+      <c r="C31" s="310"/>
+      <c r="D31" s="310"/>
+      <c r="E31" s="310"/>
+      <c r="F31" s="310"/>
+      <c r="G31" s="311"/>
       <c r="H31" s="196" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="I31" s="196"/>
     </row>
     <row r="32" spans="1:10" ht="15">
       <c r="A32" s="205" t="s">
-        <v>117</v>
+        <v>169</v>
       </c>
       <c r="B32" s="171">
         <v>0.75</v>
@@ -7072,12 +8015,12 @@
       <c r="H32" s="197"/>
       <c r="I32" s="197"/>
       <c r="J32" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30">
       <c r="A33" s="205" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="B33" s="171">
         <v>1</v>
@@ -7098,7 +8041,7 @@
     </row>
     <row r="34" spans="1:10" ht="30">
       <c r="A34" s="205" t="s">
-        <v>120</v>
+        <v>172</v>
       </c>
       <c r="B34" s="171">
         <v>0</v>
@@ -7117,12 +8060,12 @@
       <c r="H34" s="197"/>
       <c r="I34" s="197"/>
       <c r="J34" s="1" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15">
       <c r="A35" s="205" t="s">
-        <v>122</v>
+        <v>174</v>
       </c>
       <c r="B35" s="171">
         <v>0</v>
@@ -7141,12 +8084,12 @@
       <c r="H35" s="197"/>
       <c r="I35" s="197"/>
       <c r="J35" t="s">
-        <v>123</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15">
       <c r="A36" s="205" t="s">
-        <v>124</v>
+        <v>176</v>
       </c>
       <c r="B36" s="171">
         <v>0.5</v>
@@ -7165,12 +8108,12 @@
       <c r="H36" s="197"/>
       <c r="I36" s="197"/>
       <c r="J36" t="s">
-        <v>125</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="60">
       <c r="A37" s="205" t="s">
-        <v>126</v>
+        <v>178</v>
       </c>
       <c r="B37" s="171">
         <v>0</v>
@@ -7189,12 +8132,12 @@
       <c r="H37" s="197"/>
       <c r="I37" s="197"/>
       <c r="J37" s="1" t="s">
-        <v>127</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30">
       <c r="A38" s="207" t="s">
-        <v>128</v>
+        <v>180</v>
       </c>
       <c r="B38" s="171">
         <v>0</v>
@@ -7213,12 +8156,12 @@
       <c r="H38" s="197"/>
       <c r="I38" s="197"/>
       <c r="J38" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="60">
       <c r="A39" s="207" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="B39" s="171">
         <v>0</v>
@@ -7237,12 +8180,12 @@
       <c r="H39" s="197"/>
       <c r="I39" s="197"/>
       <c r="J39" s="1" t="s">
-        <v>131</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15">
       <c r="A40" s="207" t="s">
-        <v>132</v>
+        <v>184</v>
       </c>
       <c r="B40" s="171">
         <v>1</v>
@@ -7263,7 +8206,7 @@
     </row>
     <row r="41" spans="1:10" ht="15">
       <c r="A41" s="209" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="B41" s="181">
         <f>SUMPRODUCT(B32:B40,C32:C40)</f>
@@ -7293,23 +8236,23 @@
       <c r="I41" s="197"/>
     </row>
     <row r="42" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A42" s="292" t="s">
-        <v>133</v>
-      </c>
-      <c r="B42" s="293"/>
-      <c r="C42" s="293"/>
-      <c r="D42" s="293"/>
-      <c r="E42" s="293"/>
-      <c r="F42" s="293"/>
-      <c r="G42" s="294"/>
+      <c r="A42" s="309" t="s">
+        <v>185</v>
+      </c>
+      <c r="B42" s="310"/>
+      <c r="C42" s="310"/>
+      <c r="D42" s="310"/>
+      <c r="E42" s="310"/>
+      <c r="F42" s="310"/>
+      <c r="G42" s="311"/>
       <c r="H42" s="196" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I42" s="196"/>
     </row>
     <row r="43" spans="1:10" ht="30">
       <c r="A43" s="210" t="s">
-        <v>134</v>
+        <v>186</v>
       </c>
       <c r="B43" s="178">
         <v>1</v>
@@ -7330,10 +8273,10 @@
     </row>
     <row r="44" spans="1:10" ht="30">
       <c r="A44" s="207" t="s">
-        <v>135</v>
+        <v>187</v>
       </c>
       <c r="B44" s="171">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C44" s="163">
         <v>4</v>
@@ -7349,12 +8292,12 @@
       <c r="H44" s="197"/>
       <c r="I44" s="197"/>
       <c r="J44" t="s">
-        <v>136</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="45">
       <c r="A45" s="205" t="s">
-        <v>137</v>
+        <v>189</v>
       </c>
       <c r="B45" s="283">
         <v>1</v>
@@ -7375,11 +8318,11 @@
     </row>
     <row r="46" spans="1:10" ht="15">
       <c r="A46" s="212" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="B46" s="187">
         <f>SUMPRODUCT(B43:B45,C43:C45)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C46" s="165">
         <f>SUM(C43:C45)</f>
@@ -7405,25 +8348,25 @@
       <c r="I46" s="197"/>
     </row>
     <row r="47" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A47" s="292" t="s">
+      <c r="A47" s="309" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="293"/>
-      <c r="C47" s="293"/>
-      <c r="D47" s="293"/>
-      <c r="E47" s="293"/>
-      <c r="F47" s="293"/>
-      <c r="G47" s="294"/>
+      <c r="B47" s="310"/>
+      <c r="C47" s="310"/>
+      <c r="D47" s="310"/>
+      <c r="E47" s="310"/>
+      <c r="F47" s="310"/>
+      <c r="G47" s="311"/>
       <c r="H47" s="196"/>
       <c r="I47" s="196"/>
     </row>
     <row r="48" spans="1:10" ht="15">
       <c r="A48" s="214" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
       <c r="B48" s="190">
         <f t="shared" ref="B48:G48" si="0">B11+B17+B21+B25+B30+B41+B46</f>
-        <v>51.85</v>
+        <v>53.85</v>
       </c>
       <c r="C48" s="191">
         <f t="shared" si="0"/>
@@ -7450,23 +8393,23 @@
     </row>
     <row r="49" spans="1:9" ht="15">
       <c r="A49" s="216" t="s">
-        <v>139</v>
-      </c>
-      <c r="B49" s="295">
+        <v>191</v>
+      </c>
+      <c r="B49" s="312">
         <f>B48/C48</f>
-        <v>0.51849999999999996</v>
-      </c>
-      <c r="C49" s="295"/>
-      <c r="D49" s="296">
+        <v>0.53849999999999998</v>
+      </c>
+      <c r="C49" s="312"/>
+      <c r="D49" s="313">
         <f>D48/E48</f>
         <v>0</v>
       </c>
-      <c r="E49" s="296"/>
-      <c r="F49" s="297">
+      <c r="E49" s="313"/>
+      <c r="F49" s="314">
         <f>F48/G48</f>
         <v>0</v>
       </c>
-      <c r="G49" s="298"/>
+      <c r="G49" s="315"/>
       <c r="H49" s="201"/>
       <c r="I49" s="201"/>
     </row>
@@ -7530,949 +8473,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A54262-C76A-40FE-9AF3-642EF9B2EA00}">
-  <dimension ref="A1:G61"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="73" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="89.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18.75">
-      <c r="A1" s="321" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="322"/>
-      <c r="C1" s="322"/>
-      <c r="D1" s="322"/>
-      <c r="E1" s="322"/>
-      <c r="F1" s="322"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="218"/>
-      <c r="B2" s="218"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="219"/>
-    </row>
-    <row r="3" spans="1:7" ht="18.75">
-      <c r="A3" s="321" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="322"/>
-      <c r="C3" s="322"/>
-      <c r="D3" s="322"/>
-      <c r="E3" s="322"/>
-      <c r="F3" s="322"/>
-    </row>
-    <row r="5" spans="1:7" ht="23.25">
-      <c r="A5" s="323" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="323"/>
-      <c r="C5" s="323"/>
-      <c r="D5" s="323"/>
-      <c r="E5" s="323"/>
-      <c r="F5" s="323"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="220" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="324" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" s="324"/>
-      <c r="D6" s="324"/>
-      <c r="E6" s="324"/>
-      <c r="F6" s="325"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="221" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" s="222" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="222" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="222" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="222" t="s">
-        <v>143</v>
-      </c>
-      <c r="F7" s="223" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="224" t="s">
-        <v>144</v>
-      </c>
-      <c r="B8" s="225">
-        <v>1</v>
-      </c>
-      <c r="C8" s="225">
-        <v>0.75</v>
-      </c>
-      <c r="D8" s="225">
-        <v>16</v>
-      </c>
-      <c r="E8" s="225">
-        <f t="shared" ref="E8:E13" si="0">B8*C8*D8</f>
-        <v>12</v>
-      </c>
-      <c r="F8" s="284" t="s">
-        <v>145</v>
-      </c>
-      <c r="G8" s="282" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="224" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="225">
-        <v>1</v>
-      </c>
-      <c r="C9" s="225">
-        <v>1</v>
-      </c>
-      <c r="D9" s="225">
-        <v>8</v>
-      </c>
-      <c r="E9" s="225">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="F9" s="285"/>
-      <c r="G9" s="282" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="224" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="225">
-        <v>0.85</v>
-      </c>
-      <c r="C10" s="225">
-        <v>1</v>
-      </c>
-      <c r="D10" s="225">
-        <v>10</v>
-      </c>
-      <c r="E10" s="225">
-        <f t="shared" si="0"/>
-        <v>8.5</v>
-      </c>
-      <c r="F10" s="285" t="s">
-        <v>148</v>
-      </c>
-      <c r="G10" s="282" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="105">
-      <c r="A11" s="224" t="s">
-        <v>149</v>
-      </c>
-      <c r="B11" s="225">
-        <v>0.65</v>
-      </c>
-      <c r="C11" s="225">
-        <v>0.75</v>
-      </c>
-      <c r="D11" s="225">
-        <v>12</v>
-      </c>
-      <c r="E11" s="225">
-        <f t="shared" si="0"/>
-        <v>5.8500000000000005</v>
-      </c>
-      <c r="F11" s="284" t="s">
-        <v>150</v>
-      </c>
-      <c r="G11" s="282" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="120">
-      <c r="A12" s="224" t="s">
-        <v>151</v>
-      </c>
-      <c r="B12" s="225">
-        <v>0.65</v>
-      </c>
-      <c r="C12" s="225">
-        <v>0.5</v>
-      </c>
-      <c r="D12" s="225">
-        <v>10</v>
-      </c>
-      <c r="E12" s="225">
-        <f t="shared" si="0"/>
-        <v>3.25</v>
-      </c>
-      <c r="F12" s="284" t="s">
-        <v>152</v>
-      </c>
-      <c r="G12" s="282" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30">
-      <c r="A13" s="224" t="s">
-        <v>153</v>
-      </c>
-      <c r="B13" s="225">
-        <v>1</v>
-      </c>
-      <c r="C13" s="225">
-        <v>1</v>
-      </c>
-      <c r="D13" s="225">
-        <v>12</v>
-      </c>
-      <c r="E13" s="225">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="F13" s="284" t="s">
-        <v>154</v>
-      </c>
-      <c r="G13" s="282" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45">
-      <c r="A14" s="224" t="s">
-        <v>155</v>
-      </c>
-      <c r="B14" s="225">
-        <v>0.8</v>
-      </c>
-      <c r="C14" s="225">
-        <v>1</v>
-      </c>
-      <c r="D14" s="225">
-        <v>12</v>
-      </c>
-      <c r="E14" s="225">
-        <f t="shared" ref="E14:E16" si="1">B14*C14*D14</f>
-        <v>9.6000000000000014</v>
-      </c>
-      <c r="F14" s="284" t="s">
-        <v>156</v>
-      </c>
-      <c r="G14" s="282" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="224" t="s">
-        <v>157</v>
-      </c>
-      <c r="B15" s="225">
-        <v>0.9</v>
-      </c>
-      <c r="C15" s="225">
-        <v>1</v>
-      </c>
-      <c r="D15" s="225">
-        <v>10</v>
-      </c>
-      <c r="E15" s="225">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="F15" s="285" t="s">
-        <v>158</v>
-      </c>
-      <c r="G15" s="282" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="224" t="s">
-        <v>159</v>
-      </c>
-      <c r="B16" s="225">
-        <v>1</v>
-      </c>
-      <c r="C16" s="225">
-        <v>0.75</v>
-      </c>
-      <c r="D16" s="225">
-        <v>10</v>
-      </c>
-      <c r="E16" s="225">
-        <f t="shared" si="1"/>
-        <v>7.5</v>
-      </c>
-      <c r="F16" s="285" t="s">
-        <v>160</v>
-      </c>
-      <c r="G16" s="282" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="226" t="s">
-        <v>161</v>
-      </c>
-      <c r="B17" s="326"/>
-      <c r="C17" s="326"/>
-      <c r="D17" s="286">
-        <f>SUM(D8:D16)</f>
-        <v>100</v>
-      </c>
-      <c r="E17" s="278">
-        <f>SUM(E8:E16)/D17 - E19*D19 - E18*D18</f>
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="F17" s="227"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="228" t="s">
-        <v>162</v>
-      </c>
-      <c r="D18" s="229">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="228" t="s">
-        <v>163</v>
-      </c>
-      <c r="D19" s="229">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="23.25">
-      <c r="A20" s="327" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="328"/>
-      <c r="C20" s="328"/>
-      <c r="D20" s="328"/>
-      <c r="E20" s="328"/>
-      <c r="F20" s="329"/>
-    </row>
-    <row r="21" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A21" s="238" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="313"/>
-      <c r="C21" s="314"/>
-      <c r="D21" s="314"/>
-      <c r="E21" s="314"/>
-      <c r="F21" s="315"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="238" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="230" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="230" t="s">
-        <v>142</v>
-      </c>
-      <c r="D22" s="230" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="230" t="s">
-        <v>143</v>
-      </c>
-      <c r="F22" s="239" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="238" t="s">
-        <v>164</v>
-      </c>
-      <c r="B23" s="252"/>
-      <c r="C23" s="252"/>
-      <c r="D23" s="230">
-        <v>12</v>
-      </c>
-      <c r="E23" s="230">
-        <f>B23*C23*D23</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="239"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="238" t="s">
-        <v>165</v>
-      </c>
-      <c r="B24" s="252"/>
-      <c r="C24" s="252"/>
-      <c r="D24" s="230">
-        <v>8</v>
-      </c>
-      <c r="E24" s="230">
-        <f>B24*C24*D24</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="239"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="238" t="s">
-        <v>166</v>
-      </c>
-      <c r="B25" s="252"/>
-      <c r="C25" s="252"/>
-      <c r="D25" s="230">
-        <v>8</v>
-      </c>
-      <c r="E25" s="230">
-        <f>B25*C25*D25</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="239"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="238" t="s">
-        <v>167</v>
-      </c>
-      <c r="B26" s="252"/>
-      <c r="C26" s="252"/>
-      <c r="D26" s="230">
-        <v>4</v>
-      </c>
-      <c r="E26" s="230">
-        <f>B26*C26*D26</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="239"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="238" t="s">
-        <v>168</v>
-      </c>
-      <c r="B27" s="252"/>
-      <c r="C27" s="252"/>
-      <c r="D27" s="230">
-        <v>5</v>
-      </c>
-      <c r="E27" s="230">
-        <f>B27*C27*D27</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="239"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="238" t="s">
-        <v>169</v>
-      </c>
-      <c r="B28" s="252"/>
-      <c r="C28" s="252"/>
-      <c r="D28" s="230">
-        <v>5</v>
-      </c>
-      <c r="E28" s="230">
-        <f t="shared" ref="E28:E38" si="2">B28*C28*D28</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="239"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="238" t="s">
-        <v>170</v>
-      </c>
-      <c r="B29" s="252"/>
-      <c r="C29" s="252"/>
-      <c r="D29" s="230">
-        <v>14</v>
-      </c>
-      <c r="E29" s="230">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="239"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="238" t="s">
-        <v>171</v>
-      </c>
-      <c r="B30" s="252"/>
-      <c r="C30" s="252"/>
-      <c r="D30" s="230">
-        <v>6</v>
-      </c>
-      <c r="E30" s="230">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="239"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="238" t="s">
-        <v>172</v>
-      </c>
-      <c r="B31" s="252"/>
-      <c r="C31" s="252"/>
-      <c r="D31" s="230">
-        <v>8</v>
-      </c>
-      <c r="E31" s="230">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="239"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="238" t="s">
-        <v>173</v>
-      </c>
-      <c r="B32" s="252"/>
-      <c r="C32" s="252"/>
-      <c r="D32" s="230">
-        <v>4</v>
-      </c>
-      <c r="E32" s="230">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="239"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="238" t="s">
-        <v>174</v>
-      </c>
-      <c r="B33" s="252"/>
-      <c r="C33" s="252"/>
-      <c r="D33" s="230">
-        <v>4</v>
-      </c>
-      <c r="E33" s="230">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="239"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="251" t="s">
-        <v>175</v>
-      </c>
-      <c r="B34" s="252"/>
-      <c r="C34" s="252"/>
-      <c r="D34" s="252">
-        <v>6</v>
-      </c>
-      <c r="E34" s="230">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="253"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="251" t="s">
-        <v>176</v>
-      </c>
-      <c r="B35" s="252"/>
-      <c r="C35" s="252"/>
-      <c r="D35" s="252">
-        <v>6</v>
-      </c>
-      <c r="E35" s="230">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="253"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="251" t="s">
-        <v>177</v>
-      </c>
-      <c r="B36" s="252"/>
-      <c r="C36" s="252"/>
-      <c r="D36" s="252">
-        <v>4</v>
-      </c>
-      <c r="E36" s="230">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="253"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="251" t="s">
-        <v>178</v>
-      </c>
-      <c r="B37" s="252"/>
-      <c r="C37" s="252"/>
-      <c r="D37" s="252">
-        <v>4</v>
-      </c>
-      <c r="E37" s="230">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="253"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="251" t="s">
-        <v>179</v>
-      </c>
-      <c r="B38" s="252"/>
-      <c r="C38" s="252"/>
-      <c r="D38" s="252">
-        <v>2</v>
-      </c>
-      <c r="E38" s="230">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F38" s="253"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="240" t="s">
-        <v>161</v>
-      </c>
-      <c r="B39" s="241"/>
-      <c r="C39" s="262"/>
-      <c r="D39" s="262">
-        <f>SUM(D23:D38)</f>
-        <v>100</v>
-      </c>
-      <c r="E39" s="242">
-        <f>SUM(E23:E38)/D39 -E40*D40 -E41*D41-E42*D42</f>
-        <v>0</v>
-      </c>
-      <c r="F39" s="243"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="231" t="s">
-        <v>162</v>
-      </c>
-      <c r="C40" s="264"/>
-      <c r="D40" s="263">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="231" t="s">
-        <v>163</v>
-      </c>
-      <c r="D41" s="232">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="231" t="s">
-        <v>180</v>
-      </c>
-      <c r="D42" s="233">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="23.25">
-      <c r="A43" s="316" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="317"/>
-      <c r="C43" s="317"/>
-      <c r="D43" s="317"/>
-      <c r="E43" s="317"/>
-      <c r="F43" s="318"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="244" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="319"/>
-      <c r="C44" s="319"/>
-      <c r="D44" s="319"/>
-      <c r="E44" s="319"/>
-      <c r="F44" s="320"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="245" t="s">
-        <v>141</v>
-      </c>
-      <c r="B45" s="234" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" s="234" t="s">
-        <v>142</v>
-      </c>
-      <c r="D45" s="234" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" s="234" t="s">
-        <v>143</v>
-      </c>
-      <c r="F45" s="246" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="247" t="s">
-        <v>181</v>
-      </c>
-      <c r="B46" s="235"/>
-      <c r="C46" s="235"/>
-      <c r="D46" s="235">
-        <v>5</v>
-      </c>
-      <c r="E46" s="235">
-        <f t="shared" ref="E46:E52" si="3">B46*C46*D46</f>
-        <v>0</v>
-      </c>
-      <c r="F46" s="246"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="247" t="s">
-        <v>182</v>
-      </c>
-      <c r="B47" s="235"/>
-      <c r="C47" s="235"/>
-      <c r="D47" s="235">
-        <v>10</v>
-      </c>
-      <c r="E47" s="235">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F47" s="248"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="247" t="s">
-        <v>183</v>
-      </c>
-      <c r="B48" s="235"/>
-      <c r="C48" s="235"/>
-      <c r="D48" s="235">
-        <v>8</v>
-      </c>
-      <c r="E48" s="235">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F48" s="246"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="247" t="s">
-        <v>184</v>
-      </c>
-      <c r="B49" s="235"/>
-      <c r="C49" s="235"/>
-      <c r="D49" s="235">
-        <v>6</v>
-      </c>
-      <c r="E49" s="235">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F49" s="248"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="247" t="s">
-        <v>185</v>
-      </c>
-      <c r="B50" s="235"/>
-      <c r="C50" s="235"/>
-      <c r="D50" s="235">
-        <v>6</v>
-      </c>
-      <c r="E50" s="235">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F50" s="246"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="247" t="s">
-        <v>186</v>
-      </c>
-      <c r="B51" s="235"/>
-      <c r="C51" s="235"/>
-      <c r="D51" s="235">
-        <v>15</v>
-      </c>
-      <c r="E51" s="235">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F51" s="246"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="247" t="s">
-        <v>187</v>
-      </c>
-      <c r="B52" s="235"/>
-      <c r="C52" s="235"/>
-      <c r="D52" s="235">
-        <v>8</v>
-      </c>
-      <c r="E52" s="235">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F52" s="246"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="247" t="s">
-        <v>188</v>
-      </c>
-      <c r="B53" s="255"/>
-      <c r="C53" s="255"/>
-      <c r="D53" s="235">
-        <v>12</v>
-      </c>
-      <c r="E53" s="235">
-        <f t="shared" ref="E53:E57" si="4">B53*C53*D53</f>
-        <v>0</v>
-      </c>
-      <c r="F53" s="246"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="259" t="s">
-        <v>189</v>
-      </c>
-      <c r="B54" s="257"/>
-      <c r="C54" s="257"/>
-      <c r="D54" s="254">
-        <v>12</v>
-      </c>
-      <c r="E54" s="235">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F54" s="256"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="259" t="s">
-        <v>190</v>
-      </c>
-      <c r="B55" s="257"/>
-      <c r="C55" s="257"/>
-      <c r="D55" s="254">
-        <v>12</v>
-      </c>
-      <c r="E55" s="235">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F55" s="256"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="259" t="s">
-        <v>191</v>
-      </c>
-      <c r="B56" s="257"/>
-      <c r="C56" s="257"/>
-      <c r="D56" s="254">
-        <v>4</v>
-      </c>
-      <c r="E56" s="235">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F56" s="256"/>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="259" t="s">
-        <v>179</v>
-      </c>
-      <c r="B57" s="257"/>
-      <c r="C57" s="257"/>
-      <c r="D57" s="254">
-        <v>2</v>
-      </c>
-      <c r="E57" s="235">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F57" s="256"/>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="260" t="s">
-        <v>161</v>
-      </c>
-      <c r="B58" s="258"/>
-      <c r="C58" s="258"/>
-      <c r="D58" s="261">
-        <f>SUM(D46:D57)</f>
-        <v>100</v>
-      </c>
-      <c r="E58" s="249">
-        <f>SUM(E46:E57)/D58 - D59*E59  - D60*E60 - D61*E61</f>
-        <v>0</v>
-      </c>
-      <c r="F58" s="250"/>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="236" t="s">
-        <v>162</v>
-      </c>
-      <c r="D59" s="232">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="236" t="s">
-        <v>163</v>
-      </c>
-      <c r="D60" s="232">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="237" t="s">
-        <v>180</v>
-      </c>
-      <c r="D61" s="233">
-        <v>0.05</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A20:F20"/>
-  </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B17 B46:B57" xr:uid="{CC44C972-8B8F-4678-BAEB-D51FFB0200E2}">
-      <formula1>0</formula1>
-      <formula2>1</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C16 C18 C46:C57" xr:uid="{DCFB5783-098F-4837-84E1-A329359B138C}">
-      <formula1>"0,0.25,0.50,0.75,1"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E19 E41 E60" xr:uid="{301E7E41-CD71-4A91-B881-91EF87706901}">
-      <formula1>0</formula1>
-      <formula2>1</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>